<commit_message>
added search fuctionality using Ai
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>API CONTRACT FOR MEDI MENTOR</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>https://newsdata.io/api/1/news?apikey=API_KEY=health&amp;country=in&amp;language=en,hi&amp;category=health</t>
+  </si>
+  <si>
+    <t>SearchBar Doctor</t>
+  </si>
+  <si>
+    <t>To search Doctor by , name , department , profession, symptom</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/doctors/searchdoctor?query={value}</t>
   </si>
 </sst>
 </file>
@@ -224,11 +233,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="17"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -522,38 +531,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="87.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="101.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="129.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -722,8 +731,25 @@
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="8" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -744,8 +770,9 @@
     <hyperlink ref="E4" r:id="rId6"/>
     <hyperlink ref="E9" r:id="rId7"/>
     <hyperlink ref="E10" r:id="rId8"/>
+    <hyperlink ref="E11" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
appointment  added with APi contract
all  Api 's are tested initially ... report if any bug appear
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>API CONTRACT FOR MEDI MENTOR</t>
   </si>
@@ -77,18 +77,6 @@
     <t>GET</t>
   </si>
   <si>
-    <t>http://localhost:8080/appointments/getapp</t>
-  </si>
-  <si>
-    <t>To Get All Appointment</t>
-  </si>
-  <si>
-    <t>To Get Patient Details  by searching  appointment Id</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/appointments/search/{Appointment ID}</t>
-  </si>
-  <si>
     <t>get User</t>
   </si>
   <si>
@@ -144,6 +132,51 @@
   </si>
   <si>
     <t>http://localhost:8080/doctors/searchdoctor?query={value}</t>
+  </si>
+  <si>
+    <t>Get Appointment According to user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esuring that only loggedin user can see their booked /current appointment </t>
+  </si>
+  <si>
+    <t>http://localhost:8080/appointments/current/{userid}</t>
+  </si>
+  <si>
+    <t>get full details according to the appoointment id</t>
+  </si>
+  <si>
+    <t>when click on see details the in the frontend the appointment details will be shown</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/appointments/seedetails/{appointment_Id}</t>
+  </si>
+  <si>
+    <t>past appointment history according to user</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/appointments/history/{userid}</t>
+  </si>
+  <si>
+    <t>to get previous booked appointment</t>
+  </si>
+  <si>
+    <t>to get total doctor number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to get no of doctors </t>
+  </si>
+  <si>
+    <t>http://localhost:8080/doctors/totaldoctors</t>
+  </si>
+  <si>
+    <t>to get total user number</t>
+  </si>
+  <si>
+    <t>to get no of users</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/doctors/totalusers</t>
   </si>
 </sst>
 </file>
@@ -233,11 +266,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="17"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -531,38 +564,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="73.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="87.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="101.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="129.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="91.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="106.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="135.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -581,10 +614,10 @@
         <v>3</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -604,10 +637,10 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -615,16 +648,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -644,10 +677,10 @@
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -671,17 +704,17 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>13</v>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -689,16 +722,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>20</v>
+      <c r="E8" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -706,16 +739,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -723,16 +756,16 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>36</v>
+      <c r="E10" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -740,16 +773,67 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -765,14 +849,17 @@
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E5" r:id="rId2"/>
     <hyperlink ref="E6" r:id="rId3"/>
-    <hyperlink ref="E7" r:id="rId4"/>
-    <hyperlink ref="E8" r:id="rId5"/>
-    <hyperlink ref="E4" r:id="rId6"/>
+    <hyperlink ref="E4" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
     <hyperlink ref="E9" r:id="rId7"/>
     <hyperlink ref="E10" r:id="rId8"/>
     <hyperlink ref="E11" r:id="rId9"/>
+    <hyperlink ref="E12" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId11"/>
+    <hyperlink ref="E14" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated control of appointment
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Full Stack projects\healthcare-platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\healthcare-platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>API CONTRACT FOR MEDI MENTOR</t>
   </si>
@@ -143,15 +143,6 @@
     <t>http://localhost:8080/appointments/current/{userid}</t>
   </si>
   <si>
-    <t>get full details according to the appoointment id</t>
-  </si>
-  <si>
-    <t>when click on see details the in the frontend the appointment details will be shown</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/appointments/seedetails/{appointment_Id}</t>
-  </si>
-  <si>
     <t>past appointment history according to user</t>
   </si>
   <si>
@@ -177,6 +168,24 @@
   </si>
   <si>
     <t>http://localhost:8080/doctors/totalusers</t>
+  </si>
+  <si>
+    <t>patientName ,
+patientContact ,
+gender ,
+age ,
+title ,
+desc ,
+expectedDate ,
+patientAddress ,
+disease ,
+mode ,
+doctorId ,
+userId ,
+email</t>
+  </si>
+  <si>
+    <t>userId</t>
   </si>
 </sst>
 </file>
@@ -222,15 +231,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -238,12 +252,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,11 +295,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="17"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -564,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,19 +615,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -699,6 +731,9 @@
       <c r="E6" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -730,7 +765,7 @@
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -751,7 +786,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -767,44 +802,50 @@
       <c r="E10" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>45</v>
@@ -817,30 +858,13 @@
       </c>
       <c r="E13" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:L1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:F10">
+  <conditionalFormatting sqref="F2:F9">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Body">
       <formula>NOT(ISERROR(SEARCH("Body",F2)))</formula>
     </cfRule>
@@ -857,7 +881,7 @@
     <hyperlink ref="E11" r:id="rId9"/>
     <hyperlink ref="E12" r:id="rId10"/>
     <hyperlink ref="E13" r:id="rId11"/>
-    <hyperlink ref="E14" r:id="rId12"/>
+    <hyperlink ref="F11" r:id="rId12" display="vscode-file://vscode-app/c:/Users/anura/AppData/Local/Programs/Microsoft VS Code/resources/app/out/vs/code/electron-sandbox/workbench/workbench.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>

<commit_message>
dashboard api for appointment list and  approval api for approving the appointment
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
   <si>
     <t>API CONTRACT FOR MEDI MENTOR</t>
   </si>
@@ -186,6 +186,39 @@
   </si>
   <si>
     <t>userId</t>
+  </si>
+  <si>
+    <t>Doc Dash See appointment list</t>
+  </si>
+  <si>
+    <t>the doctor can see the appointment list only to the given doctor</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/appointments/docapp/{doctorID}</t>
+  </si>
+  <si>
+    <t>Update Api to Approve the appointment</t>
+  </si>
+  <si>
+    <t>api used to approve the appointment</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/appointments/approve/{appointment ID}</t>
+  </si>
+  <si>
+    <t>DoctorID</t>
+  </si>
+  <si>
+    <t>all appointment details</t>
+  </si>
+  <si>
+    <t>Appointment ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change the state from pending to approved </t>
   </si>
 </sst>
 </file>
@@ -298,11 +331,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="17"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -596,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,19 +648,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
@@ -822,7 +855,7 @@
       <c r="E11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>49</v>
       </c>
     </row>
@@ -858,6 +891,46 @@
       </c>
       <c r="E13" s="6" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -882,8 +955,10 @@
     <hyperlink ref="E12" r:id="rId10"/>
     <hyperlink ref="E13" r:id="rId11"/>
     <hyperlink ref="F11" r:id="rId12" display="vscode-file://vscode-app/c:/Users/anura/AppData/Local/Programs/Microsoft VS Code/resources/app/out/vs/code/electron-sandbox/workbench/workbench.html"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+    <hyperlink ref="E15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>